<commit_message>
Cambios excel y moment por date
Adición de etiqueta faltante y actualización excel con todos los datos
</commit_message>
<xml_diff>
--- a/reports/Planning-Template.xlsx
+++ b/reports/Planning-Template.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E2122F24-BC61-40AB-AE4D-A80C66E536E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA10A74-65FA-4E0D-A981-6A6FEE54FA4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="hidden" xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8880" firstSheet="2" activeTab="2" xr2:uid="{683E09B8-1D94-4905-B116-9D998A46AAA3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{683E09B8-1D94-4905-B116-9D998A46AAA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Copyright" sheetId="10" r:id="rId1"/>
@@ -27,8 +32,7 @@
     <definedName name="Student">Internal!$D$26:$G$26</definedName>
     <definedName name="Tester">Internal!$D$30:$I$30</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1761,9 +1765,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CF3CD5-8D08-494F-856F-AF84E30F468A}">
   <dimension ref="B2:P110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1833,7 +1837,7 @@
       </c>
       <c r="E6" s="35">
         <f>SUM(N11:N110)</f>
-        <v>3666.25</v>
+        <v>3660</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -1854,7 +1858,7 @@
       </c>
       <c r="E7" s="36">
         <f>SUM(O11:O110)</f>
-        <v>405</v>
+        <v>590</v>
       </c>
       <c r="J7" s="37"/>
     </row>
@@ -2038,10 +2042,10 @@
         <v>30</v>
       </c>
       <c r="E13" s="43" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F13" s="43" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="G13" s="44" t="s">
         <v>37</v>
@@ -2065,11 +2069,11 @@
       </c>
       <c r="N13" s="45">
         <f>IF(ISBLANK(L13), "", L13*VLOOKUP($F13,Internal!$B$26:$C$32,2,FALSE))</f>
-        <v>12.5</v>
+        <v>6.25</v>
       </c>
       <c r="O13" s="45">
         <f>IF(ISBLANK(M13), "", M13*VLOOKUP($F13,Internal!$B$26:$C$32,2,FALSE))</f>
-        <v>12.5</v>
+        <v>6.25</v>
       </c>
       <c r="P13" s="44" t="s">
         <v>38</v>
@@ -2099,10 +2103,12 @@
       <c r="I14" s="46">
         <v>46069.4375</v>
       </c>
-      <c r="J14" s="46"/>
+      <c r="J14" s="46">
+        <v>46075.875</v>
+      </c>
       <c r="K14" s="45" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>Completed</v>
       </c>
       <c r="L14" s="47">
         <v>0.5</v>
@@ -2134,7 +2140,7 @@
         <v>43</v>
       </c>
       <c r="E15" s="43" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F15" s="43" t="s">
         <v>44</v>
@@ -2390,23 +2396,29 @@
         <v>49</v>
       </c>
       <c r="H20" s="43"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
+      <c r="I20" s="46">
+        <v>46069.916666666664</v>
+      </c>
+      <c r="J20" s="46">
+        <v>46069.979166666664</v>
+      </c>
       <c r="K20" s="45" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>Completed</v>
       </c>
       <c r="L20" s="47">
         <v>2</v>
       </c>
-      <c r="M20" s="47"/>
+      <c r="M20" s="47">
+        <v>1.5</v>
+      </c>
       <c r="N20" s="45">
         <f>IF(ISBLANK(L20), "", L20*VLOOKUP($F20,Internal!$B$26:$C$32,2,FALSE))</f>
         <v>50</v>
       </c>
-      <c r="O20" s="45" t="str">
+      <c r="O20" s="45">
         <f>IF(ISBLANK(M20), "", M20*VLOOKUP($F20,Internal!$B$26:$C$32,2,FALSE))</f>
-        <v/>
+        <v>37.5</v>
       </c>
       <c r="P20" s="44" t="s">
         <v>57</v>
@@ -2433,23 +2445,29 @@
         <v>49</v>
       </c>
       <c r="H21" s="43"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
+      <c r="I21" s="46">
+        <v>46074.6875</v>
+      </c>
+      <c r="J21" s="46">
+        <v>46075.9375</v>
+      </c>
       <c r="K21" s="45" t="str">
         <f t="shared" ref="K21:K24" ca="1" si="1">IF(OR(I21="",J21=""),"",IF(AND(J21&lt;&gt;"",I21&gt;=NOW()),"Planned",IF(AND(J21&lt;&gt;"",J21&lt;NOW()),"Completed","Ongoing")))</f>
-        <v/>
+        <v>Completed</v>
       </c>
       <c r="L21" s="47">
         <v>2</v>
       </c>
-      <c r="M21" s="47"/>
+      <c r="M21" s="47">
+        <v>2</v>
+      </c>
       <c r="N21" s="45">
         <f>IF(ISBLANK(L21), "", L21*VLOOKUP($F21,Internal!$B$26:$C$32,2,FALSE))</f>
         <v>50</v>
       </c>
-      <c r="O21" s="45" t="str">
+      <c r="O21" s="45">
         <f>IF(ISBLANK(M21), "", M21*VLOOKUP($F21,Internal!$B$26:$C$32,2,FALSE))</f>
-        <v/>
+        <v>50</v>
       </c>
       <c r="P21" s="44" t="s">
         <v>58</v>
@@ -2525,23 +2543,29 @@
         <v>49</v>
       </c>
       <c r="H23" s="43"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
+      <c r="I23" s="46">
+        <v>46069.736111111109</v>
+      </c>
+      <c r="J23" s="46">
+        <v>46075.5625</v>
+      </c>
       <c r="K23" s="45" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>Completed</v>
       </c>
       <c r="L23" s="47">
         <v>2</v>
       </c>
-      <c r="M23" s="47"/>
+      <c r="M23" s="47">
+        <v>2</v>
+      </c>
       <c r="N23" s="45">
         <f>IF(ISBLANK(L23), "", L23*VLOOKUP($F23,Internal!$B$26:$C$32,2,FALSE))</f>
         <v>50</v>
       </c>
-      <c r="O23" s="45" t="str">
+      <c r="O23" s="45">
         <f>IF(ISBLANK(M23), "", M23*VLOOKUP($F23,Internal!$B$26:$C$32,2,FALSE))</f>
-        <v/>
+        <v>50</v>
       </c>
       <c r="P23" s="44" t="s">
         <v>60</v>
@@ -2568,23 +2592,29 @@
         <v>49</v>
       </c>
       <c r="H24" s="43"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="46"/>
+      <c r="I24" s="46">
+        <v>46075.885416666664</v>
+      </c>
+      <c r="J24" s="46">
+        <v>46075.979166666664</v>
+      </c>
       <c r="K24" s="45" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>Completed</v>
       </c>
       <c r="L24" s="47">
         <v>2</v>
       </c>
-      <c r="M24" s="47"/>
+      <c r="M24" s="47">
+        <v>2.15</v>
+      </c>
       <c r="N24" s="45">
         <f>IF(ISBLANK(L24), "", L24*VLOOKUP($F24,Internal!$B$26:$C$32,2,FALSE))</f>
         <v>50</v>
       </c>
-      <c r="O24" s="45" t="str">
+      <c r="O24" s="45">
         <f>IF(ISBLANK(M24), "", M24*VLOOKUP($F24,Internal!$B$26:$C$32,2,FALSE))</f>
-        <v/>
+        <v>53.75</v>
       </c>
       <c r="P24" s="44" t="s">
         <v>61</v>
@@ -3296,7 +3326,7 @@
         <v>44</v>
       </c>
       <c r="G41" s="44" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H41" s="43"/>
       <c r="I41" s="46"/>
@@ -3339,7 +3369,7 @@
         <v>44</v>
       </c>
       <c r="G42" s="44" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H42" s="43"/>
       <c r="I42" s="46"/>
@@ -3382,7 +3412,7 @@
         <v>44</v>
       </c>
       <c r="G43" s="44" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H43" s="43"/>
       <c r="I43" s="46"/>
@@ -3425,7 +3455,7 @@
         <v>44</v>
       </c>
       <c r="G44" s="44" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H44" s="43"/>
       <c r="I44" s="46"/>
@@ -3468,7 +3498,7 @@
         <v>44</v>
       </c>
       <c r="G45" s="44" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H45" s="43"/>
       <c r="I45" s="46"/>
@@ -3511,7 +3541,7 @@
         <v>44</v>
       </c>
       <c r="G46" s="44" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H46" s="43"/>
       <c r="I46" s="46"/>
@@ -3554,7 +3584,7 @@
         <v>44</v>
       </c>
       <c r="G47" s="44" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H47" s="43"/>
       <c r="I47" s="46"/>
@@ -3597,7 +3627,7 @@
         <v>44</v>
       </c>
       <c r="G48" s="44" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H48" s="43"/>
       <c r="I48" s="46"/>
@@ -3640,7 +3670,7 @@
         <v>44</v>
       </c>
       <c r="G49" s="44" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H49" s="43"/>
       <c r="I49" s="46"/>
@@ -3683,7 +3713,7 @@
         <v>44</v>
       </c>
       <c r="G50" s="44" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H50" s="43"/>
       <c r="I50" s="46"/>

</xml_diff>